<commit_message>
Converted from referenced to static lookups
</commit_message>
<xml_diff>
--- a/src/country_codes_regimes.xlsx
+++ b/src/country_codes_regimes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="590">
   <si>
     <t>AFG</t>
   </si>
@@ -1207,6 +1207,591 @@
   </si>
   <si>
     <t>AUT</t>
+  </si>
+  <si>
+    <t>Afghanistan_AFG</t>
+  </si>
+  <si>
+    <t>Albania_ALB</t>
+  </si>
+  <si>
+    <t>Algeria_ALG</t>
+  </si>
+  <si>
+    <t>Angola_ANG</t>
+  </si>
+  <si>
+    <t>Argentina_ARG</t>
+  </si>
+  <si>
+    <t>Armenia_ARM</t>
+  </si>
+  <si>
+    <t>Australia_AUL</t>
+  </si>
+  <si>
+    <t>Austria_AUS</t>
+  </si>
+  <si>
+    <t>Azerbaijan_AZE</t>
+  </si>
+  <si>
+    <t>Baden_BAD</t>
+  </si>
+  <si>
+    <t>Bahrain_BAH</t>
+  </si>
+  <si>
+    <t>Bavaria_BAV</t>
+  </si>
+  <si>
+    <t>Belgium_BEL</t>
+  </si>
+  <si>
+    <t>Benin_BEN</t>
+  </si>
+  <si>
+    <t>Burkina Faso_BFO</t>
+  </si>
+  <si>
+    <t>Bhutan_BHU</t>
+  </si>
+  <si>
+    <t>Belarus_BLR</t>
+  </si>
+  <si>
+    <t>Bangladesh_BNG</t>
+  </si>
+  <si>
+    <t>Bolivia_BOL</t>
+  </si>
+  <si>
+    <t>Bosnia_BOS</t>
+  </si>
+  <si>
+    <t>Botswana_BOT</t>
+  </si>
+  <si>
+    <t>Brazil_BRA</t>
+  </si>
+  <si>
+    <t>Burundi_BUI</t>
+  </si>
+  <si>
+    <t>Bulgaria_BUL</t>
+  </si>
+  <si>
+    <t>Cambodia_CAM</t>
+  </si>
+  <si>
+    <t>Canada_CAN</t>
+  </si>
+  <si>
+    <t>Cameroon_CAO</t>
+  </si>
+  <si>
+    <t>Cape Verde_CAP</t>
+  </si>
+  <si>
+    <t>Central African Republic_CEN</t>
+  </si>
+  <si>
+    <t>Chad_CHA</t>
+  </si>
+  <si>
+    <t>Switzerland_SWZ</t>
+  </si>
+  <si>
+    <t>Chile_CHL</t>
+  </si>
+  <si>
+    <t>China_CHN</t>
+  </si>
+  <si>
+    <t>Colombia_COL</t>
+  </si>
+  <si>
+    <t>Comoros_COM</t>
+  </si>
+  <si>
+    <t>Congo-Brazzaville_CON</t>
+  </si>
+  <si>
+    <t>Costa Rica_COS</t>
+  </si>
+  <si>
+    <t>Croatia_CRO</t>
+  </si>
+  <si>
+    <t>Cuba_CUB</t>
+  </si>
+  <si>
+    <t>Cyprus_CYP</t>
+  </si>
+  <si>
+    <t>Czechoslovakia_CZE</t>
+  </si>
+  <si>
+    <t>Czech Republic_CZR</t>
+  </si>
+  <si>
+    <t>Denmark_DEN</t>
+  </si>
+  <si>
+    <t>Djibouti_DJI</t>
+  </si>
+  <si>
+    <t>Dominican Republic_DOM</t>
+  </si>
+  <si>
+    <t>Vietnam North_DRV</t>
+  </si>
+  <si>
+    <t>Ecuador_ECU</t>
+  </si>
+  <si>
+    <t>Egypt_EGY</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea_EQG</t>
+  </si>
+  <si>
+    <t>Eritrea_ERI</t>
+  </si>
+  <si>
+    <t>Estonia_EST</t>
+  </si>
+  <si>
+    <t>Ethiopia_ETH</t>
+  </si>
+  <si>
+    <t>Ethiopia_ETI</t>
+  </si>
+  <si>
+    <t>Timor Leste_ETM</t>
+  </si>
+  <si>
+    <t>Finland_FIN</t>
+  </si>
+  <si>
+    <t>Fiji_FJI</t>
+  </si>
+  <si>
+    <t>France_FRN</t>
+  </si>
+  <si>
+    <t>Gabon_GAB</t>
+  </si>
+  <si>
+    <t>Gambia_GAM</t>
+  </si>
+  <si>
+    <t>Gran Colombia_GCL</t>
+  </si>
+  <si>
+    <t>Germany East_GDR</t>
+  </si>
+  <si>
+    <t>Ghana_GHA</t>
+  </si>
+  <si>
+    <t>Germany_GMY</t>
+  </si>
+  <si>
+    <t>Germany West_GFR</t>
+  </si>
+  <si>
+    <t>Prussia_GMY</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau_GNB</t>
+  </si>
+  <si>
+    <t>Greece_GRC</t>
+  </si>
+  <si>
+    <t>Georgia_GRG</t>
+  </si>
+  <si>
+    <t>Guatemala_GUA</t>
+  </si>
+  <si>
+    <t>Guinea_GUI</t>
+  </si>
+  <si>
+    <t>Guyana_GUY</t>
+  </si>
+  <si>
+    <t>Haiti_HAI</t>
+  </si>
+  <si>
+    <t>Honduras_HON</t>
+  </si>
+  <si>
+    <t>Hungary_HUN</t>
+  </si>
+  <si>
+    <t>India_IND</t>
+  </si>
+  <si>
+    <t>Indonesia_INS</t>
+  </si>
+  <si>
+    <t>Ireland_IRE</t>
+  </si>
+  <si>
+    <t>Iran_IRN</t>
+  </si>
+  <si>
+    <t>Iraq_IRQ</t>
+  </si>
+  <si>
+    <t>Israel_ISR</t>
+  </si>
+  <si>
+    <t>Italy_ITA</t>
+  </si>
+  <si>
+    <t>Cote D'Ivoire_IVO</t>
+  </si>
+  <si>
+    <t>Jamaica_JAM</t>
+  </si>
+  <si>
+    <t>Jordan_JOR</t>
+  </si>
+  <si>
+    <t>Japan_JPN</t>
+  </si>
+  <si>
+    <t>Kenya_KEN</t>
+  </si>
+  <si>
+    <t>Korea_KOR</t>
+  </si>
+  <si>
+    <t>Korea South_ROK</t>
+  </si>
+  <si>
+    <t>Kosovo_KOS</t>
+  </si>
+  <si>
+    <t>Kuwait_KUW</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan_KYR</t>
+  </si>
+  <si>
+    <t>Kazakhstan_KZK</t>
+  </si>
+  <si>
+    <t>Laos_LAO</t>
+  </si>
+  <si>
+    <t>Latvia_LAT</t>
+  </si>
+  <si>
+    <t>Liberia_LBR</t>
+  </si>
+  <si>
+    <t>Lebanon_LEB</t>
+  </si>
+  <si>
+    <t>Lesotho_LES</t>
+  </si>
+  <si>
+    <t>Libya_LIB</t>
+  </si>
+  <si>
+    <t>Lithuania_LIT</t>
+  </si>
+  <si>
+    <t>Mauritania_MAA</t>
+  </si>
+  <si>
+    <t>Macedonia_MAC</t>
+  </si>
+  <si>
+    <t>Madagascar_MAG</t>
+  </si>
+  <si>
+    <t>Malaysia_MAL</t>
+  </si>
+  <si>
+    <t>Mauritius_MAS</t>
+  </si>
+  <si>
+    <t>Malawi_MAW</t>
+  </si>
+  <si>
+    <t>Mexico_MEX</t>
+  </si>
+  <si>
+    <t>Moldova_MLD</t>
+  </si>
+  <si>
+    <t>Mali_MLI</t>
+  </si>
+  <si>
+    <t>Montenegro_MNT</t>
+  </si>
+  <si>
+    <t>Modena_MOD</t>
+  </si>
+  <si>
+    <t>Mongolia_MON</t>
+  </si>
+  <si>
+    <t>Morocco_MOR</t>
+  </si>
+  <si>
+    <t>Myanmar (Burma)_MYA</t>
+  </si>
+  <si>
+    <t>Mozambique_MZM</t>
+  </si>
+  <si>
+    <t>Namibia_NAM</t>
+  </si>
+  <si>
+    <t>Nepal_NEP</t>
+  </si>
+  <si>
+    <t>New Zealand_NEW</t>
+  </si>
+  <si>
+    <t>Nicaragua_NIC</t>
+  </si>
+  <si>
+    <t>Nigeria_NIG</t>
+  </si>
+  <si>
+    <t>Niger_NIR</t>
+  </si>
+  <si>
+    <t>Norway_NOR</t>
+  </si>
+  <si>
+    <t>Netherlands_NTH</t>
+  </si>
+  <si>
+    <t>Orange Free State_OFS</t>
+  </si>
+  <si>
+    <t>Oman_OMA</t>
+  </si>
+  <si>
+    <t>Pakistan_PKS</t>
+  </si>
+  <si>
+    <t>Pakistan_PAK</t>
+  </si>
+  <si>
+    <t>Panama_PAN</t>
+  </si>
+  <si>
+    <t>Papal States_PAP</t>
+  </si>
+  <si>
+    <t>Paraguay_PAR</t>
+  </si>
+  <si>
+    <t>Peru_PER</t>
+  </si>
+  <si>
+    <t>Philippines_PHI</t>
+  </si>
+  <si>
+    <t>Parma_PMA</t>
+  </si>
+  <si>
+    <t>Papua New Guinea_PNG</t>
+  </si>
+  <si>
+    <t>Poland_POL</t>
+  </si>
+  <si>
+    <t>Portugal_POR</t>
+  </si>
+  <si>
+    <t>Korea North_PRK</t>
+  </si>
+  <si>
+    <t>Qatar_QAT</t>
+  </si>
+  <si>
+    <t>Romania_RUM</t>
+  </si>
+  <si>
+    <t>Russia_RUS</t>
+  </si>
+  <si>
+    <t>South Vietnam_RVN</t>
+  </si>
+  <si>
+    <t>Rwanda_RWA</t>
+  </si>
+  <si>
+    <t>South Africa_SAF</t>
+  </si>
+  <si>
+    <t>El Salvador_SAL</t>
+  </si>
+  <si>
+    <t>Sardinia_SAR</t>
+  </si>
+  <si>
+    <t>Saudi Arabia_SAU</t>
+  </si>
+  <si>
+    <t>Saxony_SAX</t>
+  </si>
+  <si>
+    <t>Sudan-North_SDN</t>
+  </si>
+  <si>
+    <t>Senegal_SEN</t>
+  </si>
+  <si>
+    <t>Serbia_SER</t>
+  </si>
+  <si>
+    <t>Two Sicilies_SIC</t>
+  </si>
+  <si>
+    <t>Sierra Leone_SIE</t>
+  </si>
+  <si>
+    <t>Singapore_SIN</t>
+  </si>
+  <si>
+    <t>Slovak Republic_SLO</t>
+  </si>
+  <si>
+    <t>Slovenia_SLV</t>
+  </si>
+  <si>
+    <t>Solomon Islands_SOL</t>
+  </si>
+  <si>
+    <t>Somalia_SOM</t>
+  </si>
+  <si>
+    <t>Spain_SPN</t>
+  </si>
+  <si>
+    <t>Sri Lanka_SRI</t>
+  </si>
+  <si>
+    <t>South Sudan_SSU</t>
+  </si>
+  <si>
+    <t>Sudan_SUD</t>
+  </si>
+  <si>
+    <t>Suriname_SUR</t>
+  </si>
+  <si>
+    <t>Sweden_SWD</t>
+  </si>
+  <si>
+    <t>Swaziland_SWA</t>
+  </si>
+  <si>
+    <t>Syria_SYR</t>
+  </si>
+  <si>
+    <t>Tajikistan_TAJ</t>
+  </si>
+  <si>
+    <t>Taiwan_TAW</t>
+  </si>
+  <si>
+    <t>Tanzania_TAZ</t>
+  </si>
+  <si>
+    <t>Thailand_THI</t>
+  </si>
+  <si>
+    <t>Turkmenistan_TKM</t>
+  </si>
+  <si>
+    <t>Togo_TOG</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago_TRI</t>
+  </si>
+  <si>
+    <t>Tunisia_TUN</t>
+  </si>
+  <si>
+    <t>Turkey_TUR</t>
+  </si>
+  <si>
+    <t>Tuscany_TUS</t>
+  </si>
+  <si>
+    <t>United Arab Emirates_UAE</t>
+  </si>
+  <si>
+    <t>Uganda_UGA</t>
+  </si>
+  <si>
+    <t>United Kingdom_UKG</t>
+  </si>
+  <si>
+    <t>Ukraine_UKR</t>
+  </si>
+  <si>
+    <t>United Provinces_UPC</t>
+  </si>
+  <si>
+    <t>Uruguay_URU</t>
+  </si>
+  <si>
+    <t>United States                   _USA</t>
+  </si>
+  <si>
+    <t>USSR_USR</t>
+  </si>
+  <si>
+    <t>Uzbekistan_UZB</t>
+  </si>
+  <si>
+    <t>Venezuela_VEN</t>
+  </si>
+  <si>
+    <t>Vietnam_VIE</t>
+  </si>
+  <si>
+    <t>Wuerttemburg_WRT</t>
+  </si>
+  <si>
+    <t>Yemen North_YAR</t>
+  </si>
+  <si>
+    <t>Yemen_YEM</t>
+  </si>
+  <si>
+    <t>Serbia and Montenegro_YGS</t>
+  </si>
+  <si>
+    <t>Yugoslavia_YUG</t>
+  </si>
+  <si>
+    <t>Yugoslavia_YGS</t>
+  </si>
+  <si>
+    <t>Yemen South_YPR</t>
+  </si>
+  <si>
+    <t>Congo Kinshasa_ZAI</t>
+  </si>
+  <si>
+    <t>Zambia_ZAM</t>
+  </si>
+  <si>
+    <t>Zimbabwe_ZIM</t>
   </si>
 </sst>
 </file>
@@ -2117,8 +2702,8 @@
   <dimension ref="A1:F196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B170" sqref="B170"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,9 +2747,8 @@
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="str">
-        <f t="shared" ref="D2:D33" si="0">B2&amp;"_"&amp;C2</f>
-        <v>Afghanistan_AFG</v>
+      <c r="D2" s="5" t="s">
+        <v>395</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>193</v>
@@ -2183,9 +2767,8 @@
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Albania_ALB</v>
+      <c r="D3" s="5" t="s">
+        <v>396</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>194</v>
@@ -2204,9 +2787,8 @@
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Algeria_ALG</v>
+      <c r="D4" s="5" t="s">
+        <v>397</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>195</v>
@@ -2225,9 +2807,8 @@
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Angola_ANG</v>
+      <c r="D5" s="5" t="s">
+        <v>398</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>196</v>
@@ -2246,9 +2827,8 @@
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Argentina_ARG</v>
+      <c r="D6" s="5" t="s">
+        <v>399</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>197</v>
@@ -2267,9 +2847,8 @@
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Armenia_ARM</v>
+      <c r="D7" s="5" t="s">
+        <v>400</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>198</v>
@@ -2288,9 +2867,8 @@
       <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Australia_AUL</v>
+      <c r="D8" s="5" t="s">
+        <v>401</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>199</v>
@@ -2309,9 +2887,8 @@
       <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Austria_AUS</v>
+      <c r="D9" s="5" t="s">
+        <v>402</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>200</v>
@@ -2330,9 +2907,8 @@
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Azerbaijan_AZE</v>
+      <c r="D10" s="5" t="s">
+        <v>403</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>201</v>
@@ -2351,9 +2927,8 @@
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Baden_BAD</v>
+      <c r="D11" s="5" t="s">
+        <v>404</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>202</v>
@@ -2372,9 +2947,8 @@
       <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Bahrain_BAH</v>
+      <c r="D12" s="5" t="s">
+        <v>405</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>203</v>
@@ -2393,9 +2967,8 @@
       <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Bavaria_BAV</v>
+      <c r="D13" s="5" t="s">
+        <v>406</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>204</v>
@@ -2414,9 +2987,8 @@
       <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Belgium_BEL</v>
+      <c r="D14" s="5" t="s">
+        <v>407</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>205</v>
@@ -2435,9 +3007,8 @@
       <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Benin_BEN</v>
+      <c r="D15" s="5" t="s">
+        <v>408</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>206</v>
@@ -2456,9 +3027,8 @@
       <c r="C16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Burkina Faso_BFO</v>
+      <c r="D16" s="5" t="s">
+        <v>409</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>207</v>
@@ -2477,9 +3047,8 @@
       <c r="C17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Bhutan_BHU</v>
+      <c r="D17" s="5" t="s">
+        <v>410</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>208</v>
@@ -2498,9 +3067,8 @@
       <c r="C18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Belarus_BLR</v>
+      <c r="D18" s="5" t="s">
+        <v>411</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>209</v>
@@ -2519,9 +3087,8 @@
       <c r="C19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Bangladesh_BNG</v>
+      <c r="D19" s="5" t="s">
+        <v>412</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>210</v>
@@ -2540,9 +3107,8 @@
       <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Bolivia_BOL</v>
+      <c r="D20" s="5" t="s">
+        <v>413</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>211</v>
@@ -2561,9 +3127,8 @@
       <c r="C21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Bosnia_BOS</v>
+      <c r="D21" s="5" t="s">
+        <v>414</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>212</v>
@@ -2582,9 +3147,8 @@
       <c r="C22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Botswana_BOT</v>
+      <c r="D22" s="5" t="s">
+        <v>415</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>213</v>
@@ -2603,9 +3167,8 @@
       <c r="C23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Brazil_BRA</v>
+      <c r="D23" s="5" t="s">
+        <v>416</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>214</v>
@@ -2624,9 +3187,8 @@
       <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Burundi_BUI</v>
+      <c r="D24" s="5" t="s">
+        <v>417</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>215</v>
@@ -2645,9 +3207,8 @@
       <c r="C25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Bulgaria_BUL</v>
+      <c r="D25" s="5" t="s">
+        <v>418</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>216</v>
@@ -2666,9 +3227,8 @@
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Cambodia_CAM</v>
+      <c r="D26" s="5" t="s">
+        <v>419</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>217</v>
@@ -2687,9 +3247,8 @@
       <c r="C27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Canada_CAN</v>
+      <c r="D27" s="5" t="s">
+        <v>420</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>218</v>
@@ -2708,9 +3267,8 @@
       <c r="C28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Cameroon_CAO</v>
+      <c r="D28" s="5" t="s">
+        <v>421</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>219</v>
@@ -2729,9 +3287,8 @@
       <c r="C29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Cape Verde_CAP</v>
+      <c r="D29" s="5" t="s">
+        <v>422</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>220</v>
@@ -2750,9 +3307,8 @@
       <c r="C30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Central African Republic_CEN</v>
+      <c r="D30" s="5" t="s">
+        <v>423</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>221</v>
@@ -2771,9 +3327,8 @@
       <c r="C31" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Chad_CHA</v>
+      <c r="D31" s="5" t="s">
+        <v>424</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>222</v>
@@ -2792,9 +3347,8 @@
       <c r="C32" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Switzerland_SWZ</v>
+      <c r="D32" s="5" t="s">
+        <v>425</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>354</v>
@@ -2813,9 +3367,8 @@
       <c r="C33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Chile_CHL</v>
+      <c r="D33" s="5" t="s">
+        <v>426</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>223</v>
@@ -2834,9 +3387,8 @@
       <c r="C34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="5" t="str">
-        <f t="shared" ref="D34:D65" si="1">B34&amp;"_"&amp;C34</f>
-        <v>China_CHN</v>
+      <c r="D34" s="5" t="s">
+        <v>427</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>224</v>
@@ -2855,9 +3407,8 @@
       <c r="C35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Colombia_COL</v>
+      <c r="D35" s="5" t="s">
+        <v>428</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>225</v>
@@ -2876,9 +3427,8 @@
       <c r="C36" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Comoros_COM</v>
+      <c r="D36" s="5" t="s">
+        <v>429</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>226</v>
@@ -2897,9 +3447,8 @@
       <c r="C37" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Congo-Brazzaville_CON</v>
+      <c r="D37" s="5" t="s">
+        <v>430</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>227</v>
@@ -2918,9 +3467,8 @@
       <c r="C38" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Costa Rica_COS</v>
+      <c r="D38" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>228</v>
@@ -2939,9 +3487,8 @@
       <c r="C39" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Croatia_CRO</v>
+      <c r="D39" s="5" t="s">
+        <v>432</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>229</v>
@@ -2960,9 +3507,8 @@
       <c r="C40" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Cuba_CUB</v>
+      <c r="D40" s="5" t="s">
+        <v>433</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>230</v>
@@ -2981,9 +3527,8 @@
       <c r="C41" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Cyprus_CYP</v>
+      <c r="D41" s="5" t="s">
+        <v>434</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>231</v>
@@ -3002,9 +3547,8 @@
       <c r="C42" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Czechoslovakia_CZE</v>
+      <c r="D42" s="5" t="s">
+        <v>435</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>233</v>
@@ -3023,9 +3567,8 @@
       <c r="C43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Czech Republic_CZR</v>
+      <c r="D43" s="5" t="s">
+        <v>436</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>233</v>
@@ -3044,9 +3587,8 @@
       <c r="C44" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Denmark_DEN</v>
+      <c r="D44" s="5" t="s">
+        <v>437</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>234</v>
@@ -3065,9 +3607,8 @@
       <c r="C45" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Djibouti_DJI</v>
+      <c r="D45" s="5" t="s">
+        <v>438</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>235</v>
@@ -3086,9 +3627,8 @@
       <c r="C46" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Dominican Republic_DOM</v>
+      <c r="D46" s="5" t="s">
+        <v>439</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>236</v>
@@ -3107,9 +3647,8 @@
       <c r="C47" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D47" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Vietnam North_DRV</v>
+      <c r="D47" s="5" t="s">
+        <v>440</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>237</v>
@@ -3128,9 +3667,8 @@
       <c r="C48" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Ecuador_ECU</v>
+      <c r="D48" s="5" t="s">
+        <v>441</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>238</v>
@@ -3149,9 +3687,8 @@
       <c r="C49" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Egypt_EGY</v>
+      <c r="D49" s="5" t="s">
+        <v>442</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>239</v>
@@ -3170,9 +3707,8 @@
       <c r="C50" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Equatorial Guinea_EQG</v>
+      <c r="D50" s="5" t="s">
+        <v>443</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>240</v>
@@ -3191,9 +3727,8 @@
       <c r="C51" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Eritrea_ERI</v>
+      <c r="D51" s="5" t="s">
+        <v>444</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>241</v>
@@ -3212,9 +3747,8 @@
       <c r="C52" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Estonia_EST</v>
+      <c r="D52" s="5" t="s">
+        <v>445</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>242</v>
@@ -3233,9 +3767,8 @@
       <c r="C53" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Ethiopia_ETH</v>
+      <c r="D53" s="5" t="s">
+        <v>446</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>243</v>
@@ -3254,9 +3787,8 @@
       <c r="C54" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Ethiopia_ETI</v>
+      <c r="D54" s="5" t="s">
+        <v>447</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>243</v>
@@ -3275,9 +3807,8 @@
       <c r="C55" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D55" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Timor Leste_ETM</v>
+      <c r="D55" s="5" t="s">
+        <v>448</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>244</v>
@@ -3296,9 +3827,8 @@
       <c r="C56" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Finland_FIN</v>
+      <c r="D56" s="5" t="s">
+        <v>449</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>245</v>
@@ -3317,9 +3847,8 @@
       <c r="C57" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D57" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Fiji_FJI</v>
+      <c r="D57" s="5" t="s">
+        <v>450</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>246</v>
@@ -3338,9 +3867,8 @@
       <c r="C58" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D58" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>France_FRN</v>
+      <c r="D58" s="5" t="s">
+        <v>451</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>247</v>
@@ -3359,9 +3887,8 @@
       <c r="C59" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D59" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Gabon_GAB</v>
+      <c r="D59" s="5" t="s">
+        <v>452</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>248</v>
@@ -3380,9 +3907,8 @@
       <c r="C60" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D60" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Gambia_GAM</v>
+      <c r="D60" s="5" t="s">
+        <v>453</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>249</v>
@@ -3401,9 +3927,8 @@
       <c r="C61" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D61" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Gran Colombia_GCL</v>
+      <c r="D61" s="5" t="s">
+        <v>454</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>250</v>
@@ -3422,9 +3947,8 @@
       <c r="C62" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D62" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Germany East_GDR</v>
+      <c r="D62" s="5" t="s">
+        <v>455</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>251</v>
@@ -3443,9 +3967,8 @@
       <c r="C63" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Ghana_GHA</v>
+      <c r="D63" s="5" t="s">
+        <v>456</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>253</v>
@@ -3464,9 +3987,8 @@
       <c r="C64" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D64" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Germany_GMY</v>
+      <c r="D64" s="5" t="s">
+        <v>457</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>255</v>
@@ -3485,9 +4007,8 @@
       <c r="C65" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D65" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Germany West_GFR</v>
+      <c r="D65" s="5" t="s">
+        <v>458</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>255</v>
@@ -3506,9 +4027,8 @@
       <c r="C66" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D66" s="5" t="str">
-        <f t="shared" ref="D66:D97" si="2">B66&amp;"_"&amp;C66</f>
-        <v>Prussia_GMY</v>
+      <c r="D66" s="5" t="s">
+        <v>459</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>255</v>
@@ -3527,9 +4047,8 @@
       <c r="C67" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Guinea-Bissau_GNB</v>
+      <c r="D67" s="5" t="s">
+        <v>460</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>256</v>
@@ -3548,9 +4067,8 @@
       <c r="C68" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Greece_GRC</v>
+      <c r="D68" s="5" t="s">
+        <v>461</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>257</v>
@@ -3569,9 +4087,8 @@
       <c r="C69" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D69" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Georgia_GRG</v>
+      <c r="D69" s="5" t="s">
+        <v>462</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>258</v>
@@ -3590,9 +4107,8 @@
       <c r="C70" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D70" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Guatemala_GUA</v>
+      <c r="D70" s="5" t="s">
+        <v>463</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>259</v>
@@ -3611,9 +4127,8 @@
       <c r="C71" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D71" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Guinea_GUI</v>
+      <c r="D71" s="5" t="s">
+        <v>464</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>260</v>
@@ -3632,9 +4147,8 @@
       <c r="C72" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D72" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Guyana_GUY</v>
+      <c r="D72" s="5" t="s">
+        <v>465</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>261</v>
@@ -3653,9 +4167,8 @@
       <c r="C73" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D73" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Haiti_HAI</v>
+      <c r="D73" s="5" t="s">
+        <v>466</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>262</v>
@@ -3674,9 +4187,8 @@
       <c r="C74" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D74" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Honduras_HON</v>
+      <c r="D74" s="5" t="s">
+        <v>467</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>263</v>
@@ -3695,9 +4207,8 @@
       <c r="C75" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D75" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Hungary_HUN</v>
+      <c r="D75" s="5" t="s">
+        <v>468</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>264</v>
@@ -3716,9 +4227,8 @@
       <c r="C76" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>India_IND</v>
+      <c r="D76" s="5" t="s">
+        <v>469</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>265</v>
@@ -3737,9 +4247,8 @@
       <c r="C77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D77" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Indonesia_INS</v>
+      <c r="D77" s="5" t="s">
+        <v>470</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>266</v>
@@ -3758,9 +4267,8 @@
       <c r="C78" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D78" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Ireland_IRE</v>
+      <c r="D78" s="5" t="s">
+        <v>471</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>267</v>
@@ -3779,9 +4287,8 @@
       <c r="C79" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D79" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Iran_IRN</v>
+      <c r="D79" s="5" t="s">
+        <v>472</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>268</v>
@@ -3800,9 +4307,8 @@
       <c r="C80" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D80" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Iraq_IRQ</v>
+      <c r="D80" s="5" t="s">
+        <v>473</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>269</v>
@@ -3821,9 +4327,8 @@
       <c r="C81" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D81" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Israel_ISR</v>
+      <c r="D81" s="5" t="s">
+        <v>474</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>270</v>
@@ -3842,9 +4347,8 @@
       <c r="C82" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Italy_ITA</v>
+      <c r="D82" s="5" t="s">
+        <v>475</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>271</v>
@@ -3863,9 +4367,8 @@
       <c r="C83" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D83" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Cote D'Ivoire_IVO</v>
+      <c r="D83" s="5" t="s">
+        <v>476</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>272</v>
@@ -3884,9 +4387,8 @@
       <c r="C84" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D84" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Jamaica_JAM</v>
+      <c r="D84" s="5" t="s">
+        <v>477</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>273</v>
@@ -3905,9 +4407,8 @@
       <c r="C85" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D85" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Jordan_JOR</v>
+      <c r="D85" s="5" t="s">
+        <v>478</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>274</v>
@@ -3926,9 +4427,8 @@
       <c r="C86" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D86" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Japan_JPN</v>
+      <c r="D86" s="5" t="s">
+        <v>479</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>275</v>
@@ -3947,9 +4447,8 @@
       <c r="C87" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D87" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Kenya_KEN</v>
+      <c r="D87" s="5" t="s">
+        <v>480</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>276</v>
@@ -3968,9 +4467,8 @@
       <c r="C88" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D88" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Korea_KOR</v>
+      <c r="D88" s="5" t="s">
+        <v>481</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>277</v>
@@ -3989,9 +4487,8 @@
       <c r="C89" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D89" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Korea South_ROK</v>
+      <c r="D89" s="5" t="s">
+        <v>482</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>327</v>
@@ -4010,9 +4507,8 @@
       <c r="C90" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D90" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Kosovo_KOS</v>
+      <c r="D90" s="5" t="s">
+        <v>483</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>278</v>
@@ -4031,9 +4527,8 @@
       <c r="C91" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D91" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Kuwait_KUW</v>
+      <c r="D91" s="5" t="s">
+        <v>484</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>279</v>
@@ -4052,9 +4547,8 @@
       <c r="C92" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D92" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Kyrgyzstan_KYR</v>
+      <c r="D92" s="5" t="s">
+        <v>485</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>280</v>
@@ -4073,9 +4567,8 @@
       <c r="C93" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D93" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Kazakhstan_KZK</v>
+      <c r="D93" s="5" t="s">
+        <v>486</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>281</v>
@@ -4094,9 +4587,8 @@
       <c r="C94" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D94" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Laos_LAO</v>
+      <c r="D94" s="5" t="s">
+        <v>487</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>282</v>
@@ -4115,9 +4607,8 @@
       <c r="C95" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D95" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Latvia_LAT</v>
+      <c r="D95" s="5" t="s">
+        <v>488</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>283</v>
@@ -4136,9 +4627,8 @@
       <c r="C96" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D96" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Liberia_LBR</v>
+      <c r="D96" s="5" t="s">
+        <v>489</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>284</v>
@@ -4157,9 +4647,8 @@
       <c r="C97" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D97" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>Lebanon_LEB</v>
+      <c r="D97" s="5" t="s">
+        <v>490</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>285</v>
@@ -4178,9 +4667,8 @@
       <c r="C98" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D98" s="5" t="str">
-        <f t="shared" ref="D98:D129" si="3">B98&amp;"_"&amp;C98</f>
-        <v>Lesotho_LES</v>
+      <c r="D98" s="5" t="s">
+        <v>491</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>286</v>
@@ -4199,9 +4687,8 @@
       <c r="C99" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D99" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Libya_LIB</v>
+      <c r="D99" s="5" t="s">
+        <v>492</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>287</v>
@@ -4220,9 +4707,8 @@
       <c r="C100" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D100" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Lithuania_LIT</v>
+      <c r="D100" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>288</v>
@@ -4241,9 +4727,8 @@
       <c r="C101" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D101" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Mauritania_MAA</v>
+      <c r="D101" s="5" t="s">
+        <v>494</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>289</v>
@@ -4262,9 +4747,8 @@
       <c r="C102" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D102" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Macedonia_MAC</v>
+      <c r="D102" s="5" t="s">
+        <v>495</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>290</v>
@@ -4283,9 +4767,8 @@
       <c r="C103" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D103" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Madagascar_MAG</v>
+      <c r="D103" s="5" t="s">
+        <v>496</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>291</v>
@@ -4304,9 +4787,8 @@
       <c r="C104" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D104" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Malaysia_MAL</v>
+      <c r="D104" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>292</v>
@@ -4325,9 +4807,8 @@
       <c r="C105" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D105" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Mauritius_MAS</v>
+      <c r="D105" s="5" t="s">
+        <v>498</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>293</v>
@@ -4346,9 +4827,8 @@
       <c r="C106" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D106" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Malawi_MAW</v>
+      <c r="D106" s="5" t="s">
+        <v>499</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>294</v>
@@ -4367,9 +4847,8 @@
       <c r="C107" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D107" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Mexico_MEX</v>
+      <c r="D107" s="5" t="s">
+        <v>500</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>295</v>
@@ -4388,9 +4867,8 @@
       <c r="C108" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D108" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Moldova_MLD</v>
+      <c r="D108" s="5" t="s">
+        <v>501</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>296</v>
@@ -4409,9 +4887,8 @@
       <c r="C109" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D109" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Mali_MLI</v>
+      <c r="D109" s="5" t="s">
+        <v>502</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>297</v>
@@ -4430,9 +4907,8 @@
       <c r="C110" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D110" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Montenegro_MNT</v>
+      <c r="D110" s="5" t="s">
+        <v>503</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>298</v>
@@ -4451,9 +4927,8 @@
       <c r="C111" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D111" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Modena_MOD</v>
+      <c r="D111" s="5" t="s">
+        <v>504</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>299</v>
@@ -4472,9 +4947,8 @@
       <c r="C112" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D112" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Mongolia_MON</v>
+      <c r="D112" s="5" t="s">
+        <v>505</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>300</v>
@@ -4493,9 +4967,8 @@
       <c r="C113" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D113" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Morocco_MOR</v>
+      <c r="D113" s="5" t="s">
+        <v>506</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>301</v>
@@ -4514,9 +4987,8 @@
       <c r="C114" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D114" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Myanmar (Burma)_MYA</v>
+      <c r="D114" s="5" t="s">
+        <v>507</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>302</v>
@@ -4535,9 +5007,8 @@
       <c r="C115" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D115" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Mozambique_MZM</v>
+      <c r="D115" s="5" t="s">
+        <v>508</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>303</v>
@@ -4556,9 +5027,8 @@
       <c r="C116" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D116" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Namibia_NAM</v>
+      <c r="D116" s="5" t="s">
+        <v>509</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>304</v>
@@ -4577,9 +5047,8 @@
       <c r="C117" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D117" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Nepal_NEP</v>
+      <c r="D117" s="5" t="s">
+        <v>510</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>305</v>
@@ -4598,9 +5067,8 @@
       <c r="C118" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D118" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>New Zealand_NEW</v>
+      <c r="D118" s="5" t="s">
+        <v>511</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>306</v>
@@ -4619,9 +5087,8 @@
       <c r="C119" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D119" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Nicaragua_NIC</v>
+      <c r="D119" s="5" t="s">
+        <v>512</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>307</v>
@@ -4640,9 +5107,8 @@
       <c r="C120" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D120" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Nigeria_NIG</v>
+      <c r="D120" s="5" t="s">
+        <v>513</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>308</v>
@@ -4661,9 +5127,8 @@
       <c r="C121" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D121" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Niger_NIR</v>
+      <c r="D121" s="5" t="s">
+        <v>514</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>309</v>
@@ -4682,9 +5147,8 @@
       <c r="C122" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D122" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Norway_NOR</v>
+      <c r="D122" s="5" t="s">
+        <v>515</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>310</v>
@@ -4703,9 +5167,8 @@
       <c r="C123" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D123" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Netherlands_NTH</v>
+      <c r="D123" s="5" t="s">
+        <v>516</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>311</v>
@@ -4724,9 +5187,8 @@
       <c r="C124" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D124" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Orange Free State_OFS</v>
+      <c r="D124" s="5" t="s">
+        <v>517</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>312</v>
@@ -4745,9 +5207,8 @@
       <c r="C125" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D125" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Oman_OMA</v>
+      <c r="D125" s="5" t="s">
+        <v>518</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>313</v>
@@ -4766,9 +5227,8 @@
       <c r="C126" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="D126" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Pakistan_PKS</v>
+      <c r="D126" s="5" t="s">
+        <v>519</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>314</v>
@@ -4787,9 +5247,8 @@
       <c r="C127" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D127" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Pakistan_PAK</v>
+      <c r="D127" s="5" t="s">
+        <v>520</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>314</v>
@@ -4808,9 +5267,8 @@
       <c r="C128" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D128" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Panama_PAN</v>
+      <c r="D128" s="5" t="s">
+        <v>521</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>315</v>
@@ -4829,9 +5287,8 @@
       <c r="C129" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D129" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>Papal States_PAP</v>
+      <c r="D129" s="5" t="s">
+        <v>522</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>316</v>
@@ -4850,9 +5307,8 @@
       <c r="C130" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D130" s="5" t="str">
-        <f t="shared" ref="D130:D161" si="4">B130&amp;"_"&amp;C130</f>
-        <v>Paraguay_PAR</v>
+      <c r="D130" s="5" t="s">
+        <v>523</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>317</v>
@@ -4871,9 +5327,8 @@
       <c r="C131" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D131" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Peru_PER</v>
+      <c r="D131" s="5" t="s">
+        <v>524</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>318</v>
@@ -4892,9 +5347,8 @@
       <c r="C132" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D132" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Philippines_PHI</v>
+      <c r="D132" s="5" t="s">
+        <v>525</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>319</v>
@@ -4913,9 +5367,8 @@
       <c r="C133" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D133" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Parma_PMA</v>
+      <c r="D133" s="5" t="s">
+        <v>526</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>321</v>
@@ -4934,9 +5387,8 @@
       <c r="C134" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D134" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Papua New Guinea_PNG</v>
+      <c r="D134" s="5" t="s">
+        <v>527</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>322</v>
@@ -4955,9 +5407,8 @@
       <c r="C135" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D135" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Poland_POL</v>
+      <c r="D135" s="5" t="s">
+        <v>528</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>323</v>
@@ -4976,9 +5427,8 @@
       <c r="C136" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D136" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Portugal_POR</v>
+      <c r="D136" s="5" t="s">
+        <v>529</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>324</v>
@@ -4997,9 +5447,8 @@
       <c r="C137" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D137" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Korea North_PRK</v>
+      <c r="D137" s="5" t="s">
+        <v>530</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>325</v>
@@ -5018,9 +5467,8 @@
       <c r="C138" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D138" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Qatar_QAT</v>
+      <c r="D138" s="5" t="s">
+        <v>531</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>326</v>
@@ -5039,9 +5487,8 @@
       <c r="C139" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D139" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Romania_RUM</v>
+      <c r="D139" s="5" t="s">
+        <v>532</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>328</v>
@@ -5060,9 +5507,8 @@
       <c r="C140" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D140" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Russia_RUS</v>
+      <c r="D140" s="5" t="s">
+        <v>533</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>329</v>
@@ -5081,9 +5527,8 @@
       <c r="C141" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D141" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>South Vietnam_RVN</v>
+      <c r="D141" s="5" t="s">
+        <v>534</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>330</v>
@@ -5102,9 +5547,8 @@
       <c r="C142" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D142" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Rwanda_RWA</v>
+      <c r="D142" s="5" t="s">
+        <v>535</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>331</v>
@@ -5123,9 +5567,8 @@
       <c r="C143" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D143" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>South Africa_SAF</v>
+      <c r="D143" s="5" t="s">
+        <v>536</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>332</v>
@@ -5144,9 +5587,8 @@
       <c r="C144" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D144" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>El Salvador_SAL</v>
+      <c r="D144" s="5" t="s">
+        <v>537</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>333</v>
@@ -5165,9 +5607,8 @@
       <c r="C145" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D145" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Sardinia_SAR</v>
+      <c r="D145" s="5" t="s">
+        <v>538</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>334</v>
@@ -5186,9 +5627,8 @@
       <c r="C146" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D146" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Saudi Arabia_SAU</v>
+      <c r="D146" s="5" t="s">
+        <v>539</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>335</v>
@@ -5207,9 +5647,8 @@
       <c r="C147" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D147" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Saxony_SAX</v>
+      <c r="D147" s="5" t="s">
+        <v>540</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>336</v>
@@ -5228,9 +5667,8 @@
       <c r="C148" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D148" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Sudan-North_SDN</v>
+      <c r="D148" s="5" t="s">
+        <v>541</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>350</v>
@@ -5249,9 +5687,8 @@
       <c r="C149" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D149" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Senegal_SEN</v>
+      <c r="D149" s="5" t="s">
+        <v>542</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>338</v>
@@ -5270,9 +5707,8 @@
       <c r="C150" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D150" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Serbia_SER</v>
+      <c r="D150" s="5" t="s">
+        <v>543</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>339</v>
@@ -5291,9 +5727,8 @@
       <c r="C151" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D151" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Two Sicilies_SIC</v>
+      <c r="D151" s="5" t="s">
+        <v>544</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>340</v>
@@ -5312,9 +5747,8 @@
       <c r="C152" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D152" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Sierra Leone_SIE</v>
+      <c r="D152" s="5" t="s">
+        <v>545</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>341</v>
@@ -5333,9 +5767,8 @@
       <c r="C153" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D153" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Singapore_SIN</v>
+      <c r="D153" s="5" t="s">
+        <v>546</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>342</v>
@@ -5354,9 +5787,8 @@
       <c r="C154" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D154" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Slovak Republic_SLO</v>
+      <c r="D154" s="5" t="s">
+        <v>547</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>343</v>
@@ -5375,9 +5807,8 @@
       <c r="C155" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D155" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Slovenia_SLV</v>
+      <c r="D155" s="5" t="s">
+        <v>548</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>344</v>
@@ -5396,9 +5827,8 @@
       <c r="C156" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D156" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Solomon Islands_SOL</v>
+      <c r="D156" s="5" t="s">
+        <v>549</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>345</v>
@@ -5417,9 +5847,8 @@
       <c r="C157" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D157" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Somalia_SOM</v>
+      <c r="D157" s="5" t="s">
+        <v>550</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>346</v>
@@ -5438,9 +5867,8 @@
       <c r="C158" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D158" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Spain_SPN</v>
+      <c r="D158" s="5" t="s">
+        <v>551</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>347</v>
@@ -5459,9 +5887,8 @@
       <c r="C159" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D159" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Sri Lanka_SRI</v>
+      <c r="D159" s="5" t="s">
+        <v>552</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>348</v>
@@ -5480,9 +5907,8 @@
       <c r="C160" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D160" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>South Sudan_SSU</v>
+      <c r="D160" s="5" t="s">
+        <v>553</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>349</v>
@@ -5501,9 +5927,8 @@
       <c r="C161" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D161" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Sudan_SUD</v>
+      <c r="D161" s="5" t="s">
+        <v>554</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>350</v>
@@ -5522,9 +5947,8 @@
       <c r="C162" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D162" s="5" t="str">
-        <f t="shared" ref="D162:D193" si="5">B162&amp;"_"&amp;C162</f>
-        <v>Suriname_SUR</v>
+      <c r="D162" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>351</v>
@@ -5543,9 +5967,8 @@
       <c r="C163" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D163" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Sweden_SWD</v>
+      <c r="D163" s="5" t="s">
+        <v>556</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>353</v>
@@ -5564,9 +5987,8 @@
       <c r="C164" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D164" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Swaziland_SWA</v>
+      <c r="D164" s="5" t="s">
+        <v>557</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>352</v>
@@ -5585,9 +6007,8 @@
       <c r="C165" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D165" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Syria_SYR</v>
+      <c r="D165" s="5" t="s">
+        <v>558</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>355</v>
@@ -5606,9 +6027,8 @@
       <c r="C166" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D166" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Tajikistan_TAJ</v>
+      <c r="D166" s="5" t="s">
+        <v>559</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>356</v>
@@ -5627,9 +6047,8 @@
       <c r="C167" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D167" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Taiwan_TAW</v>
+      <c r="D167" s="5" t="s">
+        <v>560</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>357</v>
@@ -5648,9 +6067,8 @@
       <c r="C168" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D168" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Tanzania_TAZ</v>
+      <c r="D168" s="5" t="s">
+        <v>561</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>358</v>
@@ -5669,9 +6087,8 @@
       <c r="C169" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D169" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Thailand_THI</v>
+      <c r="D169" s="5" t="s">
+        <v>562</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>359</v>
@@ -5690,9 +6107,8 @@
       <c r="C170" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D170" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Turkmenistan_TKM</v>
+      <c r="D170" s="5" t="s">
+        <v>563</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>360</v>
@@ -5711,9 +6127,8 @@
       <c r="C171" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D171" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Togo_TOG</v>
+      <c r="D171" s="5" t="s">
+        <v>564</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>361</v>
@@ -5732,9 +6147,8 @@
       <c r="C172" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D172" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Trinidad and Tobago_TRI</v>
+      <c r="D172" s="5" t="s">
+        <v>565</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>362</v>
@@ -5753,9 +6167,8 @@
       <c r="C173" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D173" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Tunisia_TUN</v>
+      <c r="D173" s="5" t="s">
+        <v>566</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>363</v>
@@ -5774,9 +6187,8 @@
       <c r="C174" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D174" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Turkey_TUR</v>
+      <c r="D174" s="5" t="s">
+        <v>567</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>364</v>
@@ -5795,9 +6207,8 @@
       <c r="C175" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D175" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Tuscany_TUS</v>
+      <c r="D175" s="5" t="s">
+        <v>568</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>365</v>
@@ -5816,9 +6227,8 @@
       <c r="C176" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D176" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>United Arab Emirates_UAE</v>
+      <c r="D176" s="5" t="s">
+        <v>569</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>366</v>
@@ -5837,9 +6247,8 @@
       <c r="C177" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D177" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Uganda_UGA</v>
+      <c r="D177" s="5" t="s">
+        <v>570</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>367</v>
@@ -5858,9 +6267,8 @@
       <c r="C178" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D178" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>United Kingdom_UKG</v>
+      <c r="D178" s="5" t="s">
+        <v>571</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>368</v>
@@ -5879,9 +6287,8 @@
       <c r="C179" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D179" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Ukraine_UKR</v>
+      <c r="D179" s="5" t="s">
+        <v>572</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>369</v>
@@ -5900,9 +6307,8 @@
       <c r="C180" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D180" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>United Provinces_UPC</v>
+      <c r="D180" s="5" t="s">
+        <v>573</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>370</v>
@@ -5921,9 +6327,8 @@
       <c r="C181" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="D181" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Uruguay_URU</v>
+      <c r="D181" s="5" t="s">
+        <v>574</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>371</v>
@@ -5942,9 +6347,8 @@
       <c r="C182" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D182" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>United States                   _USA</v>
+      <c r="D182" s="5" t="s">
+        <v>575</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>372</v>
@@ -5963,9 +6367,8 @@
       <c r="C183" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D183" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>USSR_USR</v>
+      <c r="D183" s="5" t="s">
+        <v>576</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>192</v>
@@ -5984,9 +6387,8 @@
       <c r="C184" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D184" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Uzbekistan_UZB</v>
+      <c r="D184" s="5" t="s">
+        <v>577</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>373</v>
@@ -6005,9 +6407,8 @@
       <c r="C185" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D185" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Venezuela_VEN</v>
+      <c r="D185" s="5" t="s">
+        <v>578</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>374</v>
@@ -6026,9 +6427,8 @@
       <c r="C186" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D186" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Vietnam_VIE</v>
+      <c r="D186" s="5" t="s">
+        <v>579</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>375</v>
@@ -6047,9 +6447,8 @@
       <c r="C187" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D187" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Wuerttemburg_WRT</v>
+      <c r="D187" s="5" t="s">
+        <v>580</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>376</v>
@@ -6068,9 +6467,8 @@
       <c r="C188" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D188" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Yemen North_YAR</v>
+      <c r="D188" s="5" t="s">
+        <v>581</v>
       </c>
       <c r="E188" s="13" t="s">
         <v>378</v>
@@ -6089,9 +6487,8 @@
       <c r="C189" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D189" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Yemen_YEM</v>
+      <c r="D189" s="5" t="s">
+        <v>582</v>
       </c>
       <c r="E189" s="12" t="s">
         <v>378</v>
@@ -6110,9 +6507,8 @@
       <c r="C190" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D190" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Serbia and Montenegro_YGS</v>
+      <c r="D190" s="5" t="s">
+        <v>583</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>379</v>
@@ -6131,9 +6527,8 @@
       <c r="C191" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D191" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Yugoslavia_YUG</v>
+      <c r="D191" s="5" t="s">
+        <v>584</v>
       </c>
       <c r="E191" s="2" t="s">
         <v>379</v>
@@ -6152,9 +6547,8 @@
       <c r="C192" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D192" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Yugoslavia_YGS</v>
+      <c r="D192" s="5" t="s">
+        <v>585</v>
       </c>
       <c r="E192" s="2" t="s">
         <v>379</v>
@@ -6173,9 +6567,8 @@
       <c r="C193" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D193" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>Yemen South_YPR</v>
+      <c r="D193" s="5" t="s">
+        <v>586</v>
       </c>
       <c r="E193" s="12" t="s">
         <v>381</v>
@@ -6194,9 +6587,8 @@
       <c r="C194" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D194" s="5" t="str">
-        <f t="shared" ref="D194:D196" si="6">B194&amp;"_"&amp;C194</f>
-        <v>Congo Kinshasa_ZAI</v>
+      <c r="D194" s="5" t="s">
+        <v>587</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>382</v>
@@ -6215,9 +6607,8 @@
       <c r="C195" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D195" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>Zambia_ZAM</v>
+      <c r="D195" s="5" t="s">
+        <v>588</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>383</v>
@@ -6236,9 +6627,8 @@
       <c r="C196" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D196" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>Zimbabwe_ZIM</v>
+      <c r="D196" s="5" t="s">
+        <v>589</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>384</v>

</xml_diff>